<commit_message>
NATURINO AND FALCOTTO added, new packing lista file
</commit_message>
<xml_diff>
--- a/packing lista.xlsx
+++ b/packing lista.xlsx
@@ -763,7 +763,7 @@
   <dimension ref="A1:AC28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="W26" sqref="W26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,10 +797,7 @@
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
-      <c r="D1" s="21">
-        <f>SUM(I12:I17)</f>
-        <v>0</v>
-      </c>
+      <c r="D1" s="21"/>
       <c r="V1" t="s">
         <v>0</v>
       </c>
@@ -946,10 +943,10 @@
       </c>
     </row>
     <row r="6" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="37"/>
-      <c r="B6" s="37"/>
-      <c r="C6" s="37"/>
-      <c r="D6" s="37"/>
+      <c r="A6" s="38"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
       <c r="E6" s="33"/>
       <c r="F6" s="37"/>
       <c r="G6" s="37"/>
@@ -994,10 +991,10 @@
       </c>
     </row>
     <row r="8" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="38"/>
-      <c r="B8" s="38"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
+      <c r="A8" s="37"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
       <c r="E8" s="33"/>
       <c r="F8" s="38"/>
       <c r="G8" s="38"/>
@@ -1186,6 +1183,9 @@
       <c r="V15" t="s">
         <v>0</v>
       </c>
+      <c r="W15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:29" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="38"/>
@@ -1438,7 +1438,6 @@
       </c>
       <c r="C27" s="13"/>
       <c r="D27" s="9">
-        <f>SUM(D7,D10,D13,D18,D20,D22)</f>
         <v>0</v>
       </c>
       <c r="E27" s="11"/>
@@ -1448,7 +1447,6 @@
       </c>
       <c r="H27" s="32"/>
       <c r="I27" s="36">
-        <f>SUM(I11,I18,I20,I22)</f>
         <v>0</v>
       </c>
       <c r="J27" s="11"/>
@@ -1458,7 +1456,6 @@
       </c>
       <c r="M27" s="16"/>
       <c r="N27" s="9">
-        <f>SUM(N19,N21)</f>
         <v>0</v>
       </c>
       <c r="O27" s="11" t="s">
@@ -1470,7 +1467,6 @@
       </c>
       <c r="R27" s="10"/>
       <c r="S27" s="9">
-        <f>SUM(S15,S21)</f>
         <v>0</v>
       </c>
       <c r="T27" s="20"/>
@@ -1495,10 +1491,7 @@
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
       <c r="K28" s="5"/>
-      <c r="L28" s="3">
-        <f>D27+I27+N27+S27</f>
-        <v>0</v>
-      </c>
+      <c r="L28" s="3"/>
       <c r="M28" s="3" t="s">
         <v>0</v>
       </c>

</xml_diff>